<commit_message>
Implementacion de Dublin Core en las tablas de metadatos
</commit_message>
<xml_diff>
--- a/data/metadatos-bga.xlsx
+++ b/data/metadatos-bga.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isabelvaldesarias/Documents/GitHub/coleccion-bga/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F28D8E7E-71C1-3E4F-8A67-3E5B1AEE58F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D345F78B-80D8-364B-ABB3-E1D4ACEFF8F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{E7F9E5F3-8C94-9649-90B9-6550F09EBEE2}"/>
+    <workbookView xWindow="19900" yWindow="1860" windowWidth="18500" windowHeight="17440" activeTab="1" xr2:uid="{E7F9E5F3-8C94-9649-90B9-6550F09EBEE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Obra" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <si>
     <t>ID</t>
   </si>
@@ -70,9 +70,6 @@
     <t>suicidas-sisga-1.jpg</t>
   </si>
   <si>
-    <t>Periódico</t>
-  </si>
-  <si>
     <t>Doble suicidio en "El Sisga"</t>
   </si>
   <si>
@@ -131,6 +128,18 @@
   </si>
   <si>
     <t>exmilitar-mata-esposa.jpg</t>
+  </si>
+  <si>
+    <t>dc.title</t>
+  </si>
+  <si>
+    <t>dc.date</t>
+  </si>
+  <si>
+    <t>dc.publisher</t>
+  </si>
+  <si>
+    <t>dc.identifier</t>
   </si>
 </sst>
 </file>
@@ -549,19 +558,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" t="s">
         <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -569,19 +578,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" t="s">
         <v>21</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>22</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>23</v>
-      </c>
-      <c r="F4" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -595,7 +604,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -609,16 +618,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="E1" t="s">
         <v>5</v>
@@ -629,16 +638,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>14</v>
-      </c>
-      <c r="E2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -646,16 +655,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
         <v>26</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -663,10 +672,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s">
         <v>28</v>
-      </c>
-      <c r="E4" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -674,10 +683,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" t="s">
         <v>30</v>
-      </c>
-      <c r="E5" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>